<commit_message>
adding adjusted script and spreadsheet
</commit_message>
<xml_diff>
--- a/outputs_citizens.xlsx
+++ b/outputs_citizens.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesle\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wkz/bclt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123D5B50-BA83-43A6-B3C3-83E016106042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ABED91-1E21-654E-86C7-F8D51858F0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="YEAR" sheetId="1" r:id="rId1"/>
+    <sheet name="2006" sheetId="2" r:id="rId1"/>
+    <sheet name="2020" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="177">
   <si>
     <t>File Name</t>
   </si>
@@ -626,7 +627,53 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
@@ -687,7 +734,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H2" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E6EF23E5-8DBA-154B-B9C5-584E5B05D637}" name="Table13" displayName="Table13" ref="A1:H2" insertRow="1" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:H2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{C8F9DBE2-87AF-B347-BE2C-79DBE8BEFEFB}" name="File Name"/>
+    <tableColumn id="2" xr3:uid="{AD8995F4-89D6-1B45-80DB-EE1118B6A4CB}" name="Date of Petition"/>
+    <tableColumn id="3" xr3:uid="{B9A4679B-7456-764E-A936-F605A8C1B764}" name="Identity of Submitting Entity"/>
+    <tableColumn id="4" xr3:uid="{71C3A7BF-68AB-0B4C-BFC9-25605CDA235A}" name="Representation Details"/>
+    <tableColumn id="5" xr3:uid="{C3E495DF-7AA0-2346-962B-AE0A06324A53}" name="Cited Statutes or Regulations"/>
+    <tableColumn id="6" xr3:uid="{FA499DC7-5E95-0A47-BDB5-93FD54FAC55A}" name="FDA Action Commented On"/>
+    <tableColumn id="7" xr3:uid="{813ECA79-141B-AC42-A087-48099A0EE7F2}" name="Requested Action"/>
+    <tableColumn id="8" xr3:uid="{F592A77F-C128-B743-9E9F-510487D63E22}" name="Justification for Request"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H2" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A1:H2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="File Name"/>
@@ -1019,26 +1083,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{910EE7AA-3F4D-7A4E-A74D-81B2E148413E}">
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1064,7 +1128,61 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1114,7 +1232,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1143,7 +1261,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1175,7 +1293,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1201,7 +1319,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1227,7 +1345,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1253,7 +1371,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -1279,7 +1397,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -1305,7 +1423,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -1331,7 +1449,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -1357,7 +1475,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -1383,7 +1501,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>102</v>
       </c>
@@ -1409,7 +1527,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>108</v>
       </c>
@@ -1435,7 +1553,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -1461,7 +1579,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -1487,7 +1605,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>130</v>
       </c>
@@ -1513,7 +1631,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>138</v>
       </c>
@@ -1539,7 +1657,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>146</v>
       </c>
@@ -1565,7 +1683,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>154</v>
       </c>
@@ -1591,7 +1709,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>162</v>
       </c>
@@ -1617,7 +1735,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>170</v>
       </c>

</xml_diff>

<commit_message>
adding 2024 for petitions
</commit_message>
<xml_diff>
--- a/outputs_citizens.xlsx
+++ b/outputs_citizens.xlsx
@@ -16119,7 +16119,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -18171,27 +18171,2337 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Not representing another entity</t>
+          <t>Not Mentioned</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>21 C.F.R. § 14.29, 21 C.F.R. § 312.32(a), 45 C.F.R. §§ 46.103(a), 46.103(b)(5)</t>
+          <t>21 CFR 14.29; 21 CFR 312.32(a); 45 CFR 46.103(a); 45 CFR 46.103(b)(5)</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Planned advisory committee meeting related to the Lykos Therapeutics New Drug Application for MDMA-Assisted Therapy</t>
+          <t>FDA's planned advisory committee meeting on the Lykos Therapeutics MDMA-Assisted Therapy New Drug Application</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Convene an advisory committee meeting on MDMA-Assisted Therapy with an extended open public hearing to include perspectives of stakeholders concerned about the Lykos NDA’s shortcomings and risks</t>
+          <t>Convene an advisory committee meeting on MDMA-Assisted Therapy with an extended Open Public Hearing prioritizing concerns about Lykos Therapeutics' application</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>The petition argues that the Lykos NDA involves a novel drug-psychotherapy hybrid, raises serious safety and efficacy concerns, lacks impartiality in trial reporting, and has significant public interest; it highlights alleged adverse event suppression and recommends cross-disciplinary expert input</t>
+          <t>Petitioner argues that the MDMA-assisted therapy application is novel and precedent-setting, involves significant safety concerns, unresolved scientific issues, and high public interest. The petitioner also raises ethical and regulatory concerns over data reporting, protocol safety, and internal culture at Lykos/MAPS, calling for independent expert input and transparency.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2150-0001_Envelope.pdf</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>04/25/2024</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Parenteral Technologies, LLC</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Michael A. Creaturo, submitting on behalf of Parenteral Technologies, LLC</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Not Mentioned</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Not Mentioned</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Not Mentioned</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Not Mentioned</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2151-0001_Citizen_Petition_from_UnidosUS.pdf</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>May 7, 2024</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>UnidosUS</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>No, UnidosUS is not representing another entity but has co-signatories from other organizations</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>5 U.S.C. § 553(e), 21 C.F.R. § 10.30, Section 403(a) of the Food, Drug, and Cosmetic Act</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Voluntary fortification policy and labeling practices for unfortified corn masa flour and products</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Require a warning label on all unfortified corn masa flour and products made with corn masa to inform consumers of the lack of folic acid and associated risk of neural tube defects</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Voluntary fortification has failed to ensure adequate folic acid intake among Hispanic women, resulting in persistent health disparities; a warning label is needed to alert consumers and drive public health improvement</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2215-0001_Citizen_Petition_from_Metaltronica_Spa.pdf</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>May 2, 2024</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Metaltronica Spa</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>No, the submitting entity is not representing another entity</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>21 CFR §10.25(a), 21 CFR §10.30, IEC 60601-1, IEC 60601-2, IEC 60601-2-28, IEC 60601-1-3, IEC 60601-2-45, IEC 62304, ISO 14971</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>FDA classification and premarket submission requirements for tomo digital mammography devices (product code OTE)</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Reclassify tomo digital mammography devices (product code OTE) from Class III (PMA) to Class II (510(k)), aligning them with Full Field Digital Mammography (FFDM) devices (product code MUE)</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>The petitioner argues that risks and necessary evidence for OTE devices are similar to those for MUE devices, both of which use ionizing radiation and share hardware/software components. The technology is mature, widely adopted globally, and supported by harmonized standards. Market data and adverse event analysis show no significant safety differences, and reclassification would reduce costs for manufacturers, regulators, and users while maintaining safety and effectiveness.</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2220-0001_Citizen_Petition_from_Encube_Ethicals_Private_Limi.pdf</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>May 6, 2024</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Encube Ethicals Private Limited</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>No, the submitting entity is not representing another entity</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>21 C.F.R. § 10.25(a), 21 C.F.R. § 10.30, 21 C.F.R. § 314.161, 21 C.F.R. § 314.122, 21 C.F.R. § 25.31(a)</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Determination of whether the Reference Listed Drug (RLD) PENNSAID (diclofenac sodium topical solution 2%) has been withdrawn for reasons of safety or effectiveness</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Determine whether PENNSAID (diclofenac sodium topical solution 2% w/w, NDA# N204623) has been withdrawn for reasons of safety or effectiveness</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>The petitioner believes the discontinuation was for commercial reasons and not related to safety or effectiveness. A determination from the FDA is required to allow referencing the RLD in an ANDA.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2242-0001_Citizen_Petition_from_David_Behar_Redacted.pdf</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>April 28, 2024</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>David Behar, M.D.</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>No, the submitting entity is not representing another entity</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>21 C.F.R. § 10.30, 21 C.F.R. § 10.40(e)(1), Administrative Procedure Act</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>FDA requirement for a prescription to obtain CPAP machines</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Make CPAP (Continuous Positive Airway Pressure) machines available over the counter without a prescription, and require sellers to provide instruction manuals at a 6th-grade reading level with illustrations</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>The petitioner argues that requiring prescriptions for CPAP machines results in high costs, delays, and limited access, contributing to untreated sleep apnea, increased healthcare costs, preventable accidents, and health disparities. The petitioner cites successful price drops following over-the-counter access to hearing aids, points to racial and economic inequities, and contends that self-diagnosis is feasible with support from sleep apps and partner observations. The petition invokes urgent public health and economic consequences to justify bypassing traditional rulemaking procedures.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2272-0001_Citizen_Petition_from_Aurobindo_Pharma_USA__Inc_.pdf</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>May 7, 2024</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Aurobindo Pharma Limited</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Blessy Johns, US Agent for Aurobindo Pharma Limited (Aurobindo Pharma USA, Inc.)</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Section 505(j) of the FDCA, 21 CFR § 10.25(a), 21 CFR § 10.30, 21 CFR § 314.122, 21 CFR § 314.161, 21 CFR § 25.31(a), 21 CFR § 25.15(d), 21 CFR § 10.30(b)</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Determination regarding whether INVEGA® (Paliperidone) Extended-Release Tablets 1.5 mg, NDA #021999, has been withdrawn for safety or effectiveness reasons</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Request the FDA to determine whether INVEGA® (Paliperidone) Extended-Release Tablets 1.5 mg has been withdrawn for reasons of safety or effectiveness</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>The petitioner notes that the drug appears in the discontinued section of the Orange Book and seeks confirmation that the discontinuation was not due to safety or effectiveness concerns in order to support an Abbreviated New Drug Application (ANDA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2314-0001_Citizen_Petition_from_Aurobindo_Pharma_USA_Inc_.pdf</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>May 9, 2024</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Aurobindo Pharma Limited</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Blessy Johns, US Agent for Aurobindo Pharma Limited (Aurobindo Pharma USA, Inc.)</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Section 505(j) of the FDCA, 21 CFR § 10.25(a), 21 CFR § 10.30, 21 CFR § 314.122, 21 CFR § 314.161, 21 CFR § 314.162, 21 CFR § 25.31(a), 21 CFR § 25.15(d), 21 CFR § 10.30(b)</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Determination regarding whether Augmentin XR (amoxicillin and clavulanate potassium) extended-release tablets, NDA 050785, has been withdrawn for reasons of safety or effectiveness</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Request the FDA to determine whether Augmentin XR (amoxicillin and clavulanate potassium) extended-release tablets, NDA 050785, has been voluntarily withdrawn from sale for reasons of safety or effectiveness</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>The petitioner notes that Augmentin XR now appears in the discontinued section of the Orange Book and requests confirmation that the withdrawal was not due to safety or effectiveness concerns, in order to support an Abbreviated New Drug Application (ANDA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2326-0001_Citizen_Petition_from_Hyman__Phelps___McNamara__P_.pdf</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>May 10, 2024</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Hyman, Phelps &amp; McNamara, P.C.</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>United Therapeutics Corporation</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>21 C.F.R. §§ 10.30 and 10.31, 21 U.S.C. §§ 355(b)(1)(A)(iv), 355(d)(3), 355(e), 351(a)(2)(B); 21 C.F.R. §§ 314.50(d), 314.105(a), 314.107(b)(4), 314.110(a), 314.125(a)(3)-(b)(1), (b)(4), (b)(13); 21 C.F.R. § 25.31(a)</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>FDA’s tentative approval of Liquidia’s section 505(b)(2) NDA for YUTREPIA</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Rescind tentative approval of Liquidia's NDA for YUTREPIA, issue a Complete Response Letter, and withhold any final approval until compliance with CGMP is ensured</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>The sole API supplier for YUTREPIA, LGM Pharma, has a history of severe and ongoing CGMP violations, and remains under a Consent Decree. These violations threaten the safety, quality, and compliance of YUTREPIA’s supply chain, and thus the product should not be approved or tentatively approved until all issues are remediated and FDA confirms compliance.</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2379-0001_Citizen_Petition_from_The_Humane_Society_of_the_Un.pdf</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>May 15, 2024</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>The Humane Society of the United States and the Humane Society Legislative Fund</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Not representing another entity; the petition is submitted on behalf of HSUS and HSLF themselves</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>21 U.S.C. § 301 et seq., 5 U.S.C. § 553(e), 21 C.F.R. § 10.30</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>FDA's regulatory policies and guidance that imply animal testing is required for drug approval</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Amend FDA regulations and guidance to clarify that animal testing is not required, issue a new guidance document detailing accepted non-animal methods (NAMs), and update all future guidance documents to reference the new NAMs guidance</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Animal testing is often unnecessary, expensive, time-consuming, and not required by law. Non-animal methods (NAMs) are more efficient, reliable, and ethical. Current FDA language creates confusion and incentivizes unnecessary animal tests, hindering drug innovation and violating Congressional intent under FDORA</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2461-0001_Citizen_Petition_from_Ho_Chunk__Inc__on_behalf_of_.pdf</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>May 17, 2024</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Ho-Chunk, Inc.</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Yes, Ho-Chunk, Inc. is submitting on behalf of Rock River Manufacturing Company</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>21 U.S.C. § 301 et seq., 21 C.F.R. § 10.30, Executive Order 13175, HHS Tribal Consultation Policy</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Requirements for Tobacco Product Manufacturing Practice (FDA-2013-N-0227), specifically part 1120</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Amend the Proposed Rule to include an exemption from part 1120 for tribally-owned cigarette manufacturers such as Rock River Manufacturing</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>The petitioner argues that the proposed rule imposes significant economic burdens on small tribal manufacturers like Rock River, threatening their viability. Rock River is one of only two tribally-owned tobacco manufacturers in the U.S., and it already operates under strict tribal regulation and high compliance standards. An exemption would allow the tribe to preserve jobs and economic activity on the Winnebago Reservation without materially affecting overall tobacco regulation.</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2482-0001_Citizen_Petition_from_Age_Reversal_Unity.pdf</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>May 7, 2024</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Age Reversal Unity</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>No, the submitting entity is not representing another entity</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>21 C.F.R. § 10.30, 21 C.F.R. § 25.32</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Lack of regulation classifying aging as a disease</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Request the FDA to promulgate a new regulation classifying aging as a disease for purposes of research, treatment, and prevention</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Aging is the primary risk factor for many chronic diseases and has identifiable biological hallmarks that are targetable. Recognizing aging as a disease could shift the healthcare paradigm to proactive aging management, increase research funding, and streamline regulatory pathways for relevant therapies.</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2513-0001_Citizen_Petition_from_Innogenix_LLC.pdf</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>May 21, 2024</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Innogenix LLC</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>No, the submitting entity is not representing another entity</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>21 C.F.R. §§ 10.25, 10.30, 314.122, 314.161; Sections 505(j) and 505(w) of the Federal Food, Drug, and Cosmetic Act</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Determination of whether the Reference Listed Drug (RLD), Flagyl® (metronidazole) Tablets 250 mg and 500 mg (NDA N012623), has been withdrawn for safety or effectiveness reasons</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Request that the FDA determine whether Flagyl® Tablets 250 mg and 500 mg, approved under NDA N012623, has been voluntarily withdrawn for safety or effectiveness reasons</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>The petitioner believes the discontinuation was due to commercial reasons and is not aware of any safety or effectiveness concerns. A determination by FDA is required to enable ANDA submissions referencing the RLD.</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2514-0001_Citizen_Petition_from_Zydus_Pharmaceuticals__USA__.pdf</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>May 22, 2024</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Zydus Pharmaceuticals (USA) Inc.</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>No, the submitting entity is not representing another entity</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>21 C.F.R. § 10.25(a), 21 C.F.R. § 10.30, 21 C.F.R. § 314.161, 21 C.F.R. § 314.122, 21 C.F.R. § 25.31(a), 21 C.F.R. § 10.30(b)</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Determination of whether the Reference Listed Drug (RLD) NUPLAZID® (pimavanserin) tablets, 17 mg (NDA# N207318) has been withdrawn for reasons of safety or effectiveness</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Request that the FDA determine whether NUPLAZID® (pimavanserin) tablets, 17 mg (NDA# N207318) has been withdrawn from commercial sale for reasons of safety or effectiveness</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>The petitioner states that NUPLAZID® 17 mg appears in the Discontinued Section of the Orange Book but is unaware of any safety or effectiveness issues. They believe the discontinuation was for commercial reasons and seek FDA’s confirmation to support an ANDA referencing the drug</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2515-0001_Citizen_Petition_from_Encube_Ethicals_Private_Limi.pdf</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>May 22, 2024</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Encube Ethicals Private Limited</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>No, the submitting entity is not representing another entity</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>21 C.F.R. § 10.25(a), 21 C.F.R. § 10.30, 21 C.F.R. § 314.161, 21 C.F.R. § 314.122, 21 C.F.R. § 25.31(a), 21 C.F.R. § 10.30(b)</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Determination of whether the Reference Listed Drug (RLD), Fortesta (testosterone) Gel (10 mg/0.5 gm Actuation, NDA# 021463), has been withdrawn for reasons of safety or effectiveness</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Request the FDA to determine whether Fortesta (testosterone) Gel (10 mg/0.5 gm Actuation, NDA# 021463) has been voluntarily withdrawn from commercial sale for safety or effectiveness reasons</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>The petitioner states that Fortesta appears in the Discontinued Section of the Orange Book but is unaware of any safety or effectiveness concerns. Believing the withdrawal was due to commercial reasons, the petitioner seeks FDA confirmation to enable an ANDA referencing the drug</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2538-0001_Suitability_Petition_from_Hyman__Phelps___McNamara.pdf</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>May 23, 2024</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Hyman, Phelps &amp; McNamara, P.C.</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Yes, the law firm is submitting the petition on behalf of a client (not named)</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) of the FDC Act, 21 C.F.R. § 314.93, 21 C.F.R. §§ 10.20 and 10.30, 21 C.F.R. § 25.31, 21 C.F.R. § 10.30(b), FDC Act § 505B(a)(1)(A)(i)</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Suitability of a new dosage form for Cetrorelix Acetate (pre-filled syringe solution) as an ANDA based on RLD CETROTIDE® (powder for reconstitution)</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Request that FDA declare Cetrorelix Acetate Injection 0.25 mg/mL pre-filled syringe suitable for submission as an ANDA</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>The proposed product is a ready-to-use form with the same active ingredient, strength, route of administration, and indications as the RLD, reducing the risk of medication error and improving ease of use. The change in dosage form does not affect safety or efficacy, and the product is not intended for pediatric patients, supporting a PREA waiver.</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2730-0001_Citizen_Petition_from_Kenneth_D__Eichenbaum.pdf</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>June 2, 2024</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Kenneth D. Eichenbaum, MD, MSE</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>No, the submitting entity is not representing another entity</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>21 C.F.R. § 10.20, 21 C.F.R. § 10.30, Section 351 of the Public Health Service Act, 21 C.F.R. § 25.30, 21 C.F.R. § 25.31, 21 C.F.R. § 10.30(b)</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>FDA’s potential action to expand the label for SRP-9001 (Elvidys, delandistrogene moxeparvovec-rokl)</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Request that the FDA refrain from authorizing an expanded label for SRP-9001 (Elvidys) and re-evaluate its limited benefit relative to associated risks</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>The petition argues that both Phase 2 and Phase 3 trials failed to meet their primary endpoints, with weak evidence of benefit and significant safety risks including liver injury, myocarditis, and immune-mediated myositis. Expanding the label may hinder the development of more promising therapies, waste resources, and damage FDA's credibility. Additional studies and alternative therapies should be prioritized.</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2752-0001_Suitability_Petition_from_Hyman__Phelps___McNamara.pdf</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>June 6, 2024</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Hyman, Phelps &amp; McNamara, P.C.</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Yes, the submitting entity is representing an unnamed client</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) of the FDC Act, 21 C.F.R. § 314.93, 21 C.F.R. §§ 10.20 and 10.30, 21 C.F.R. § 25.31, 21 C.F.R. § 10.30(b)</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Suitability determination for Bupivacaine Hydrochloride Injection, USP (pharmacy bulk package) as an ANDA referencing MARCAINE (NDA 016964)</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Request that FDA declare Bupivacaine Hydrochloride Injection, USP in pharmacy bulk packages (100 mL, 500 mL, 1L, 2L) of 0.25% and 0.5% strengths suitable for submission as an ANDA</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>The petitioner asserts that the proposed bulk packaging has the same concentration and dosage form as the RLD but offers operational advantages such as reduced waste and increased supply to mitigate drug shortages. The labeling includes necessary safety instructions and does not raise new questions of safety or efficacy, so no clinical investigations are required. The PREA requirements do not apply.</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2753-0001_Suitability_Petition_from_Hyman__Phelps___McNamara.pdf</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>June 6, 2024</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Hyman, Phelps &amp; McNamara, P.C.</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Yes, the submitting entity is representing an unnamed client</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) of the FDC Act, 21 C.F.R. § 314.93, 21 C.F.R. §§ 10.20 and 10.30, 21 C.F.R. § 25.31, 21 C.F.R. § 10.30(b), FDC Act § 505B(a)(1)(A)(i)</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Suitability determination for submission of an ANDA for a new presentation of Fentanyl Citrate Injection, USP</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Request that FDA declare Fentanyl Citrate Injection, USP, 50 mcg/mL in pharmacy bulk packages (100 mL, 500 mL, 1L, and 2L) suitable for submission as an ANDA</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>The petitioner argues that while the proposed drug differs from the RLD only in total fill volume/total drug content, the concentration and therapeutic use remain the same. Bulk packaging will reduce waste, support operational efficiencies, and help mitigate ongoing drug shortages. PREA requirements do not apply, and no clinical investigations are necessary to demonstrate safety or efficacy.</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2757-0001_Suitability_Petition_from_Hyman__Phelps___McNamara.pdf</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>June 6, 2024</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Hyman, Phelps &amp; McNamara, P.C.</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Yes, the submitting entity is representing an unnamed client</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) of the FDC Act, 21 C.F.R. § 314.93, 21 C.F.R. §§ 10.20 and 10.30, 21 C.F.R. § 25.31, 21 C.F.R. § 10.30(b), FDC Act § 505B(a)(1)(A)(i)</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Suitability determination for Oxytocin Injection, USP (synthetic), 10 USP Units/mL, for submission as an ANDA in pharmacy bulk package sizes</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Request that FDA declare Oxytocin Injection, USP (synthetic), 10 USP Units/mL, in pharmacy bulk packages (100 mL, 500 mL, 1L, and 2L) suitable for submission as an ANDA</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>The proposed product has the same concentration and intended therapeutic use as the RLD, but differs in total fill volume/total drug content. The larger volume pharmacy bulk packaging aims to reduce waste, improve operational efficiency, and help prevent potential drug shortages. No new safety or efficacy issues are raised. PREA does not apply, and FDA has approved similar petitions in the past.</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2758-0001_Suitability_Petition_from_Hyman__Phelps___McNamara.pdf</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>June 6, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Hyman, Phelps &amp; McNamara, P.C. :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Petition submitted by the law firm on behalf of an unnamed client (entity not disclosed) :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) FDC Act; 21 C.F.R. § 314.93; 21 C.F.R. §§ 10.20, 10.30; Section 505(j)(2)(A)(iii) FDC Act; 21 C.F.R. § 314.3; Section 505B(a)(1)(A)(i) FDC Act (PREA); 21 C.F.R. § 25.31; 21 C.F.R. § 10.30(b) :contentReference[oaicite:6]{index=6}:contentReference[oaicite:7]{index=7}</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>FDA’s determination of suitability for an ANDA for Ropivacaine Hydrochloride Injection in pharmacy bulk package sizes :contentReference[oaicite:8]{index=8}:contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Declare that pharmacy bulk packages (100 mL, 500 mL, 1 L, 2 L) of Ropivacaine Hydrochloride Injection (0.2 %, 0.5 %, 1 %) are suitable for submission as an ANDA :contentReference[oaicite:10]{index=10}:contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Change is limited to total fill volume/drug content while concentration, dosage, route, and labeling remain consistent with the RLD; larger bulk packages reduce waste, improve operational efficiency, lower costs, and help mitigate an ongoing drug shortage; prior FDA precedents for similar petitions; no new safety or efficacy questions; PREA not applicable; categorical environmental exclusion claimed :contentReference[oaicite:12]{index=12}:contentReference[oaicite:13]{index=13}</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2778-0001_Suitability_Petition_from_Pharmobedient_Consulting.pdf</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>June 7, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Pharmobedient Consulting, LLC :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Pharmobedient Consulting, LLC submitting on behalf of Pharmobedient Pharmaceuticals, LLC (product sponsor) :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) FDC Act; Section 505(j)(2)(C)(iii) FDC Act; 21 C.F.R. § 10.20; 21 C.F.R. § 10.30; 21 C.F.R. § 314.93; 21 C.F.R. § 25.31; Pediatric Research Equity Act (PREA) Section 505B :contentReference[oaicite:6]{index=6}:contentReference[oaicite:7]{index=7}</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>FDA’s determination of suitability for an ANDA for Chlorzoxazone Orally Disintegrating Tablets (ODT) 250 mg and 500 mg differing in dosage form from the RLD :contentReference[oaicite:8]{index=8}:contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Declare that Chlorzoxazone ODT 250 mg and 500 mg are suitable for submission in an ANDA under Section 505(j)(2)(C) :contentReference[oaicite:10]{index=10}:contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>ODT provides rapid onset without water, improves compliance for patients with swallowing difficulties, offers dosage flexibility with added 250 mg strength, aligns with existing labeling and bioequivalence to RS, raises no new safety or efficacy questions, environmental exclusion claimed, and pediatric studies waiver requested under PREA :contentReference[oaicite:12]{index=12}:contentReference[oaicite:13]{index=13}</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2779-0001_Suitability_Petition_from_Hyman__Phelps___McNamara.pdf</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>June 10, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Hyman, Phelps &amp; McNamara, P.C. :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Law firm filing on behalf of an unnamed client :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) FDC Act; Section 505(j)(2)(A)(iii) FDC Act; Section 505B(a)(1)(A)(i) FDC Act (PREA); 21 C.F.R. § 314.93; 21 C.F.R. §§ 10.20, 10.30; 21 C.F.R. § 10.33; 21 C.F.R. § 25.31 :contentReference[oaicite:6]{index=6}</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>FDA’s prior denial and determination of suitability for an ANDA for Diclofenac Potassium Tablets 12.5 mg differing in strength from the RLD CATAFLAM :contentReference[oaicite:7]{index=7}:contentReference[oaicite:8]{index=8}</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Declare Diclofenac Potassium Tablets 12.5 mg suitable for submission as an ANDA under Section 505(j) :contentReference[oaicite:9]{index=9}:contentReference[oaicite:10]{index=10}</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Proposed lower strength supports lowest effective dosing, literature and bioavailability studies show comparable safety and efficacy to higher strengths, EMA precedent confirms acceptability, no new safety or labeling concerns, PREA inapplicable, and categorical environmental exclusion claimed :contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2843-0001_Citizen_Petition_from_Zach_Richardson_Redacted.pdf</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>June 8, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Zach Richardson :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Petition filed by Zach Richardson on his own behalf; no separate represented entity :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>21 C.F.R. § 10.30; 21 C.F.R. § 10.30(b); 21 C.F.R. § 25.30; 21 C.F.R. § 25.31; Federal Food, Drug, and Cosmetic Act :contentReference[oaicite:6]{index=6}</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>FDA’s current policy of not classifying aging as a disease; petitioner seeks issuance of a new regulation to change this :contentReference[oaicite:7]{index=7}:contentReference[oaicite:8]{index=8}</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Issue a regulation classifying aging as a disease :contentReference[oaicite:9]{index=9}:contentReference[oaicite:10]{index=10}</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Aging drives most chronic diseases and economic burden; scientific evidence links biomarkers and pathways with potential interventions; recognizing aging as a disease would spur R&amp;D, improve healthspan, and reduce healthcare costs, with precedents such as obesity classification noted alongside acknowledgment of possible Social Security impacts :contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2846-0001_Petition_for_Reclassification_from_Pyrexar_Medical.pdf</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>June 6, 2024 :contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Pyrexar Medical Inc. :contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Petition filed directly by Pyrexar Medical Inc.; no separate representative entity :contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Section 513(e) of the Federal Food, Drug, and Cosmetic Act :contentReference[oaicite:7]{index=7}</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>FDA’s classification of the BSD‑2000 Hyperthermia System as a Class III medical device :contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Reclassify the BSD‑2000 Hyperthermia System from Class III to Class II under Section 513(e) :contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Extensive clinical data show the BSD‑2000’s proven safety and efficacy; years of global clinical use confirm low risk; advanced safety features and precise temperature control align with Class II expectations; reclassification would streamline access, cut regulatory costs, broaden adoption, and improve patient outcomes while matching precedents for similar devices </t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2885-0001_Suitability_Petition_from_Hyman__Phelps___McNamara.pdf</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>June 17, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Hyman, Phelps &amp; McNamara, P.C. :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Law firm submitting on behalf of an unnamed client :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) FDC Act; Section 505(j)(2)(A)(iii) FDC Act; Section 505B(a)(1)(A)(i) FDC Act (PREA); 21 C.F.R. § 314.93; 21 C.F.R. §§ 10.20, 10.30; 21 C.F.R. § 25.31 :contentReference[oaicite:6]{index=6}:contentReference[oaicite:7]{index=7}</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>FDA’s determination of suitability for an ANDA for new 200 mg and 300 mg strengths of Olaparib Tablets differing from the RLD strengths :contentReference[oaicite:8]{index=8}:contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Declare Olaparib Tablets 200 mg and 300 mg suitable for submission as an ANDA under Section 505(j) :contentReference[oaicite:10]{index=10}:contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Strengths align with RLD dosing recommendations, reduce tablet burden, raise no new safety or efficacy questions, PREA inapplicable to strength changes, and categorical environmental exclusion claimed :contentReference[oaicite:12]{index=12}:contentReference[oaicite:13]{index=13}</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2909-0001_Suitability_Petition_from_Hyman__Phelps___McNamara.pdf</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>June 17, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Hyman, Phelps &amp; McNamara, P.C. :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Law firm filing on behalf of an unnamed client :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) FDC Act; Section 505(j)(2)(A)(iii) FDC Act; 21 C.F.R. § 314.93; 21 C.F.R. §§ 10.20, 10.30; Section 505B(a)(1)(A)(i) FDC Act (PREA); 21 C.F.R. § 25.31 :contentReference[oaicite:6]{index=6}:contentReference[oaicite:7]{index=7}</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>FDA’s determination of suitability for an ANDA for new 4 mg and 12 mg Buprenorphine Sublingual Tablet strengths differing from the RLD SUBUTEX :contentReference[oaicite:8]{index=8}:contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Declare Buprenorphine Sublingual Tablets 4 mg and 12 mg suitable for submission as an ANDA under Section 505(j) :contentReference[oaicite:10]{index=10}:contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Strengths match RLD dosing guidance, reduce pill burden, introduce no new safety or efficacy concerns, PREA requirements do not apply to strength changes, and a categorical environmental exclusion is claimed :contentReference[oaicite:12]{index=12}:contentReference[oaicite:13]{index=13}</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2932-0001_Suitability_Petition_from_Newcastle_Bioscience_LLC.pdf</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>June 19, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Newcastle Bioscience LLC :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Newcastle Bioscience LLC submitting on behalf of an unnamed client :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) FDC Act; 21 C.F.R. § 10.30; 21 C.F.R. § 314.93; 21 C.F.R. § 25.31; Pediatric Research Equity Act (PREA) Section 505B; Section 505B(k) FDC Act :contentReference[oaicite:6]{index=6}:contentReference[oaicite:7]{index=7}</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>FDA’s determination of suitability for an ANDA for Rosuvastatin Calcium Orally Disintegrating Tablets (5 mg, 10 mg, 20 mg, 40 mg) differing in dosage form from the RLD Crestor Tablets :contentReference[oaicite:8]{index=8}:contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Declare Rosuvastatin Calcium Orally Disintegrating Tablets 5 mg, 10 mg, 20 mg, 40 mg suitable for submission as an ANDA under Section 505(j) :contentReference[oaicite:10]{index=10}:contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Change limited to dosage form while strengths, dosing schedule, and labeling match RLD; ODT improves patient convenience without new safety or efficacy issues; no clinical concerns raised; pediatric study waiver requested; categorical environmental exclusion claimed :contentReference[oaicite:12]{index=12}:contentReference[oaicite:13]{index=13}</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2933-0001_Citizen_Petition_from_Chobani_LLC.pdf</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>June 18, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Chobani, LLC :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Petition filed directly by Chobani, LLC; no separate represented entity :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Section 401 FDC Act; 21 C.F.R. § 131.200; 21 C.F.R. § 131.200(b); 21 C.F.R. § 101.4(b)–(c); 21 C.F.R. § 25.30; 21 C.F.R. § 25.31; 21 C.F.R. § 25.32(a) :contentReference[oaicite:6]{index=6}</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>FDA’s yogurt standard of identity at 21 C.F.R. § 131.200, which currently excludes ultrafiltered nonfat milk as a basic dairy ingredient :contentReference[oaicite:7]{index=7}:contentReference[oaicite:8]{index=8}</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Initiate rulemaking to amend 21 C.F.R. § 131.200 to include ultrafiltered nonfat milk as a basic dairy ingredient in yogurt :contentReference[oaicite:9]{index=9}:contentReference[oaicite:10]{index=10}</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Ultrafiltered nonfat milk maintains yogurt’s essential qualities, enables modern processing, offers higher protein with lower sugar/lactose, supports consumer demand for lactose‑free/high‑protein foods, harmonizes with FDA nutrition goals and international standards, and raises no new safety, environmental, or economic concerns :contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2952-0001_Citizen_Petition_from_Sarah_A__Norring___Redacted.pdf</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>June 20, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Sarah A. Norring, Ph.D. :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Petition filed by Sarah A. Norring on her own behalf; no represented entity :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>21 C.F.R. § 10.30; 21 C.F.R. § 314.161; 21 C.F.R. § 25.31 :contentReference[oaicite:6]{index=6}:contentReference[oaicite:7]{index=7}</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>FDA’s determination under 21 C.F.R. § 314.161 regarding whether the listed drug Lunelle was withdrawn for safety or effectiveness reasons :contentReference[oaicite:8]{index=8}:contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Conclude that Lunelle (estradiol cypionate/medroxyprogesterone acetate injectable) was not withdrawn from sale for safety or effectiveness reasons :contentReference[oaicite:10]{index=10}:contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Historical evidence shows only syringe recall due to potency uncertainty; vials retained full efficacy, no safety concerns cited; subsequent market withdrawal driven by manufacturing/business decisions rather than safety or effectiveness; therefore, FDA should find the withdrawal not safety‑related :contentReference[oaicite:12]{index=12}</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-2955-0001_Citizen_Petition_from_Dsquare_LLC.pdf</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>June 18, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Dsquare LLC :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Petition filed directly by Dsquare LLC; no separate represented entity :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>21 C.F.R. § 10.30; 21 C.F.R. § 201; 21 C.F.R. § 201.64; 21 C.F.R. § 201.57 :contentReference[oaicite:6]{index=6}</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Current FDA labeling policy for sodium‑containing N‑acetylcysteine drugs used in treating acetaminophen intoxication, which lacks required sodium warnings and black‑box alerts :contentReference[oaicite:7]{index=7}:contentReference[oaicite:8]{index=8}</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Amend labeling of all sodium‑containing N‑acetylcysteine products to add a high‑sodium content warning for the general population and a Black Box Warning for salt‑sensitive patients or those with cardiovascular/CNS disease :contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Recommended treatment delivers sodium doses far exceeding FDA limits; high acute sodium loads are linked to serious cardiovascular and neurological events and reported fatalities; existing FDA guidelines and the former RLD CETYLEV include such warnings, but current products do not; adding warnings will protect salt‑sensitive and general populations and align labeling with FDA safety standards :contentReference[oaicite:10]{index=10}</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3090-0001_Suitability_Petition_from_Epic_Pharma__LLC__on_beh.pdf</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>June 28, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Epic Pharma, LLC :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Epic Pharma, LLC filed the petition as Regulatory Agent on behalf of Humanwell Pharmaceutical US, Inc. :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) FD&amp;C Act; 21 C.F.R. § 314.93; 21 C.F.R. § 10.20; 21 C.F.R. § 10.30; 21 C.F.R. § 25.31; Pediatric Research Equity Act (§ 505B) :contentReference[oaicite:6]{index=6}</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>FDA’s determination of suitability for an ANDA differing in dosage form/strength from the RLD APTIOM—specifically Eslicarbazepine Acetate Oral Suspension 50 mg/mL :contentReference[oaicite:7]{index=7}:contentReference[oaicite:8]{index=8}</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Declare Eslicarbazepine Acetate Oral Suspension 50 mg/mL suitable for submission as an ANDA under § 505(j) :contentReference[oaicite:9]{index=9}:contentReference[oaicite:10]{index=10}</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Change is limited to converting APTIOM tablets to a ready‑to‑use suspension at an equivalent dosage; labeling, dosing schedule, and safety/efficacy remain unchanged; suspension aids patients who cannot swallow tablets; precedent for approving similar dosage‑form petitions; no new clinical concerns; petitioner seeks PREA waiver and claims categorical environmental exclusion :contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3188-0001_Suitability_Petition_from_Lachman_Consulting_Servi.pdf</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>July 3, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Lachman Consulting Services, Inc. :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Lachman Consulting Services, Inc. filed the petition on behalf of an unnamed client :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) FD&amp;C Act; Section 505B FD&amp;C Act (PREA); 21 C.F.R. § 10.20; 21 C.F.R. § 10.30; 21 C.F.R. § 25.31 :contentReference[oaicite:6]{index=6}:contentReference[oaicite:7]{index=7}</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>FDA’s determination of suitability for an ANDA for a new 1,250 mg/100 mL (12.5 mg/mL) strength of Levetiracetam in Sodium Chloride Injection differing from RLD strengths :contentReference[oaicite:8]{index=8}:contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Declare Levetiracetam in Sodium Chloride Injection 1,250 mg/100 mL (12.5 mg/mL) suitable for submission as an ANDA under Section 505(j) :contentReference[oaicite:10]{index=10}:contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Proposed strength is bracketed by existing RLD strengths, reduces medical waste, avoids multiple infusions or compounding, maintains same active ingredient, route, indications, and labeling, introduces no new safety or efficacy concerns, PREA deemed inapplicable, and categorical environmental exclusion claimed :contentReference[oaicite:12]{index=12}:contentReference[oaicite:13]{index=13}</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3292-0001_Suitability_Petition_from_Felix_Pharmaceuticals_Pv.pdf</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>July 10, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Felix Pharmaceuticals Pvt. Ltd. :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Petition filed directly by Felix Pharmaceuticals Pvt. Ltd.; no represented third party :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Section 512(n)(3) FD&amp;C Act; 21 C.F.R. § 25.30(h); 21 C.F.R. § 25.21 :contentReference[oaicite:6]{index=6}:contentReference[oaicite:7]{index=7}</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>FDA’s determination of suitability for an abbreviated new animal drug application (ANADA) for a Maropitant Citrate oral solution differing in dosage form from the pioneer CERENIA tablets :contentReference[oaicite:8]{index=8}:contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Declare that Maropitant Citrate Oral Solution 40 mg/mL is suitable for submission as an ANADA under Section 512(n)(3) :contentReference[oaicite:10]{index=10}:contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Only dosage‑form change—from tablet to oral solution—with same active ingredient, route, and dosage; proposed solution will be bioequivalent, uses excipients already approved for dogs, allows precise weight‑based dosing via calibrated syringes, improves ease of administration, and poses no new safety or efficacy concerns; categorical environmental exclusion claimed :contentReference[oaicite:12]{index=12}:contentReference[oaicite:13]{index=13}</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3293-0001_Suitability_Petition_from_Newcastle_Bioscience_LLC.pdf</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>July 9, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Newcastle Bioscience LLC :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Petition filed directly by Newcastle Bioscience LLC; no separate represented entity :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) FDC Act; 21 C.F.R. § 10.30; 21 C.F.R. § 25.31; Pediatric Research Equity Act (§ 505B) :contentReference[oaicite:6]{index=6}:contentReference[oaicite:7]{index=7}</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>FDA’s determination of suitability for an ANDA for Lacosamide Orally Disintegrating Tablets that differ in dosage form and strengths from the RLD Vimpat tablets :contentReference[oaicite:8]{index=8}:contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Declare Lacosamide Orally Disintegrating Tablets 25 mg, 37.5 mg, 75 mg, 112.5 mg, 125 mg, and 175 mg suitable for submission as an ANDA under Section 505(j) :contentReference[oaicite:10]{index=10}:contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>New strengths and ODT form provide flexible dosing (especially for renal/hepatic impairment and pediatrics), facilitate titration to lowest effective dose, remove need for oral solution, offer ease of administration, introduce no new safety or efficacy concerns, seek PREA waiver, and claim categorical environmental exclusion :contentReference[oaicite:12]{index=12}:contentReference[oaicite:13]{index=13}</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3357-0001_Citizen_Petition_from_Randall_Steinmeyer___Redacte.pdf</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Not stated in the petition</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Randall Steinmeyer</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>None—petitioner appears on his own behalf</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Federal Food, Drug &amp; Cosmetic Act; 21 C.F.R. Part 809 (Medical Devices; Laboratory Developed Tests)</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>FDA’s delegation of oversight for DNA paternity‑test LDTs to the American Association of Blood Banks (AABB) instead of direct regulation</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Ban LabCorp and DDC’s forged DNA paternity tests, place such tests under direct FDA regulation, remove AABB as regulator, and bar the respondents from marketing LDTs</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Tests are alleged forgeries mislabeled as paternity tests; respondents control the market, switched real tests for cheap forgeries, forged expert signatures, lied to FDA about forensic validity, and profit from fraud—creating public‑health and justice risks that require immediate FDA action</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3479-0001_Citizen_Petition_from_Jingwei_Pharmaceutical_Compa.pdf</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>July 23, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Jingwei Pharmaceutical Company, Ltd. :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Petition submitted directly by Jingwei Pharmaceutical Company, Ltd.; no separate represented entity :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>21 U.S.C. § 355; 21 C.F.R. § 10.25; 21 C.F.R. § 10.30; 21 C.F.R. § 25.30; 21 C.F.R. § 25.31 :contentReference[oaicite:6]{index=6}:contentReference[oaicite:7]{index=7}</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>FDA’s oversight and approval standards for generic drug manufacturers that use a biocatalytic process to produce sitagliptin active pharmaceutical ingredient (API) :contentReference[oaicite:8]{index=8}:contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Require such manufacturers to submit (1) a complete certificate of analysis for the biocatalyst, (2) detailed preparation process for the biocatalyst, (3) analytical protocols for residual enzymes and biological impurities, and (4) purging strategies documenting the fate of the biocatalyst :contentReference[oaicite:10]{index=10}:contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Biocatalytic processes introduce complex enzyme‑related impurities that are hard to detect and purge; inconsistent impurity profiles threaten patient safety, especially for the large diabetic population relying on sitagliptin; many generics lack necessary technology, so stricter information requirements are needed to protect public health :contentReference[oaicite:12]{index=12}:contentReference[oaicite:13]{index=13}</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3482-0001_Citizen_Petition_from_Qilu_Pharmaceutical__Hainan_.pdf</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>July 24, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Qilu Pharmaceutical (Hainan) Co., Ltd. :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Petition filed directly by Qilu Pharmaceutical (Hainan) Co., Ltd.; no separate represented entity :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Sections 505(j) and 505(w) FDC Act; 21 C.F.R. § 10.25(a); 21 C.F.R. § 10.30; 21 C.F.R. § 314.122; 21 C.F.R. § 314.161; 21 C.F.R. § 25.31 :contentReference[oaicite:6]{index=6}:contentReference[oaicite:7]{index=7}</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>FDA’s listing of JESDUVROQ (daprodustat) tablets 1 mg, 2 mg, 4 mg, 6 mg, 8 mg in the Orange Book’s Discontinued Drug Product List and the related withdrawal determination :contentReference[oaicite:8]{index=8}:contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Determine that JESDUVROQ (daprodustat) tablets 1 mg–8 mg were not withdrawn for reasons of safety or effectiveness :contentReference[oaicite:10]{index=10}:contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Petitioner is unaware of any safety or efficacy issues; believes discontinuation was solely for commercial reasons; a ‘not‑withdrawn‑for‑safety/efficacy’ finding will allow ANDA applicants to cite the drug as the RLD :contentReference[oaicite:12]{index=12}:contentReference[oaicite:13]{index=13}</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3484-0001_Petition_for_Reclassification_of_next_generation_s.pdf</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>June 28, 2024 :contentReference[oaicite:0]{index=0}:contentReference[oaicite:1]{index=1}</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Foundation Medicine, Inc. :contentReference[oaicite:2]{index=2}:contentReference[oaicite:3]{index=3}</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Petition filed directly by Foundation Medicine, Inc.; no separate represented entity :contentReference[oaicite:4]{index=4}:contentReference[oaicite:5]{index=5}</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Section 513(f)(3) FD&amp;C Act; Section 513(f)(1) FD&amp;C Act; 21 C.F.R. § 860.123; 21 C.F.R. § 860.134 :contentReference[oaicite:6]{index=6}:contentReference[oaicite:7]{index=7}</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>FDA’s current classification of next‑generation sequencing oncology panel devices (product code PQP) as Class III medical devices and its announced intent to reclassify IVDs :contentReference[oaicite:8]{index=8}:contentReference[oaicite:9]{index=9}</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Reclassify all NGS oncology panel devices with one or more companion diagnostic indications (product code PQP) from Class III to Class II (high‑risk with special controls) :contentReference[oaicite:10]{index=10}:contentReference[oaicite:11]{index=11}</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Extensive regulatory experience and published data show risks can be mitigated through rigorous special controls; reclassification would preserve safety and effectiveness while improving patient access, ensuring high‑quality genomic testing, and aligning regulation with FDA’s 2024 reclassification initiative for high‑risk IVDs :contentReference[oaicite:12]{index=12}:contentReference[oaicite:13]{index=13}</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3563-0001_Citizen_Petition_from_Hyman__Phelps___McNamara__P_.pdf</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>July 29, 2024</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Hyman, Phelps &amp; McNamara, P.C.</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Aquestive Therapeutics, Inc.</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>21 C.F.R. §§ 10.30 and 10.31; section 505(q) of the FDCA</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>FDA policy not requiring food-effect studies for intranasal products even when the active moiety has a known food effect</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Require food-effect studies for intranasal spray products where the active moiety has a known food effect when administered orally; investigate lack of efficacy for such products documented in FDA's Adverse Event Reporting System</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Intranasal products may be partially swallowed and thus subject to food effects that alter pharmacokinetics and efficacy; literature and FAERS data suggest lack of efficacy could be due to unstudied food effects; a food-effect study is simple, quick, and low-cost and could inform safe labeling and use</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3567-0001_Suitability_Petition_from_Lachman_Consulting_Servi.pdf</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>July 25, 2024</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Lachman Consulting Services, Inc.</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>A client represented by Lachman Consulting Services, Inc. (client identity not disclosed)</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) of the FD&amp;C Act; 21 C.F.R. § 10.20; 21 C.F.R. § 10.30</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>FDA's lack of approval for lower strength (25 mg, 50 mg, 100 mg) sertraline capsules despite their utility for titration, initiation, and tapering of therapy</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Declare that Sertraline Capsules, 25 mg, 50 mg, and 100 mg are suitable for submission in an Abbreviated New Drug Application (ANDA)</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>The currently approved capsule strengths (150 mg and 200 mg) do not accommodate initial titration or tapering; the proposed lower strengths would enhance dosing flexibility, improve patient adherence, reduce copays during titration, and align with approved labeling recommendations</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3571-0001_Suitability_Petition_from_Premier_Consulting.pdf</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>July 29, 2024</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Premier Research Consulting, LLC</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Premier Consulting is submitting on its own behalf; no separate represented entity is named</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) of the FD&amp;C Act; 21 CFR § 10.20; 21 CFR § 10.30; 21 CFR § 314.93</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>FDA’s current limitation of the Reference Listed Drug (LOTREL) to capsule dosage form only</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Determine that Amlodipine and Benazepril hydrochloride Oral Liquid is suitable for submission in an Abbreviated New Drug Application (ANDA)</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>The proposed product differs only in dosage form (oral liquid vs. capsule) while maintaining the same active ingredients, indication, route, and dosing regimen as the RLD; this change facilitates administration, particularly for patients with swallowing difficulties, without introducing new safety or efficacy concerns</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3573-0001_Suitability_Petition_from_Premier_Consulting.pdf</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>July 29, 2024</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Premier Research Consulting, LLC</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Premier Consulting is submitting on its own behalf; no separate represented entity is named</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) of the FD&amp;C Act; 21 CFR § 10.20; 21 CFR § 10.30; 21 CFR § 314.93</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>FDA’s limitation of the Reference Listed Drug (ZESTORETIC) to tablet dosage form</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Determine that Lisinopril and Hydrochlorothiazide Oral Liquid is suitable for submission in an Abbreviated New Drug Application (ANDA)</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>The proposed oral liquid formulation maintains the same active ingredients, dosage strengths, route of administration, and indication as the RLD ZESTORETIC; converting the dosage form from tablet to liquid facilitates administration, particularly in populations with swallowing difficulties, without introducing new safety or efficacy concerns</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3699-0001_Citizen_Petition_from_Zydus_Pharmaceuticals__USA__.pdf</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>August 2, 2024</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Zydus Pharmaceuticals (USA) Inc.</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Zydus Pharmaceuticals (USA) Inc. is submitting on its own behalf; no separate represented entity is named</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>21 C.F.R. § 10.25(a); 21 C.F.R. § 10.30; 21 C.F.R. § 314.161; 21 C.F.R. § 314.122</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Whether IC-GREEN (indocyanine green for injection, USP) 25 mg has been withdrawn from sale for safety or effectiveness reasons</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Request a determination from the FDA as to whether the Reference Listed Drug IC-GREEN 25 mg was withdrawn from sale for reasons of safety or effectiveness</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>IC-GREEN 25 mg is listed as discontinued in the FDA’s Orange Book and is no longer marketed by Renew Pharmaceuticals Ltd.; a determination is needed to clarify whether the discontinuation was due to safety or effectiveness concerns to support potential ANDA submission</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3761-0001_Citizen_Petition_from_Spark_Biomedical__Inc_.pdf</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>July 31, 2024</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Spark Biomedical, Inc.</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Spark Biomedical, Inc. is submitting on its own behalf; no separate represented entity is named</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Section 3060(a) of the 21st Century Cures Act; Section 201(h) of the FD&amp;C Act</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>FDA’s lack of enforcement on neurostimulation wellness devices making unapproved medical claims</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Enforce regulation of neurostimulation wellness products making therapeutic claims, remove non-compliant products from the market, and require amended advertising to eliminate misleading medical claims</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Neurostimulation wellness devices are being marketed with unsubstantiated claims about treating serious medical conditions without FDA approval; such devices should be regulated as medical devices under existing law to protect public health and ensure consumer safety</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3799-0001_Citizen_Petition_from_Raaha_LLC.pdf</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>August 7, 2024</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Raaha LLC</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Raaha LLC is submitting on its own behalf; no separate represented entity is named</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) of the FD&amp;C Act; 21 CFR § 10.20; 21 CFR § 10.30; 21 CFR § 314.92</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Approval of ANDAs for Prednisolone Ophthalmic Solution 1% without demonstrating long-term stability under refrigerated conditions</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Require generic applicants to submit long-term stability studies under refrigerated conditions for Prednisolone Ophthalmic Solution 1%, withhold approval of ANDAs lacking such data, and reconsider approval and rating of ANDA #216935 if it lacks these studies</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Refrigerated storage is permitted per the RLD labeling; ophthalmic suspensions are sensitive to temperature variations affecting critical quality attributes like particle size and viscosity; lack of stability data under refrigerated conditions could compromise product quality, safety, and efficacy, posing risks to public health</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3820-0001_Citizen_Petition_from_Vanguard_Regulatory_Services.pdf</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>August 9, 2024</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Vanguard Regulatory Services, Inc.</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Vanguard Regulatory Services, Inc. is submitting the petition on behalf of Nagase Viita Co., Ltd.</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>21 C.F.R. § 10.30; 21 C.F.R. § 101.9(c)(6)(i); Sections 403(q), 403(a), 201(n), and 701(a) of the FD&amp;C Act</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>FDA’s current exclusion of Isomaltodextrin (IMD) from the definition of dietary fiber under 21 C.F.R. § 101.9(c)(6)(i)</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Amend the definition of dietary fiber in 21 C.F.R. § 101.9(c)(6)(i) to include Isomaltodextrin (IMD/Fibryxa®) as an isolated or synthetic non-digestible carbohydrate with beneficial physiological effects</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Scientific studies show that IMD significantly reduces postprandial blood glucose and triglyceride levels in humans, especially in individuals with elevated responses; thus, IMD provides beneficial physiological effects and meets the criteria for inclusion as a dietary fiber under FDA regulations</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3821-0001_Cover_Letter_for_Suitability_Petition_from_Aurora_.pdf</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>August 8, 2024</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Aurora Pharmaceutical, Inc.</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Aurora Pharmaceutical, Inc. is submitting on its own behalf; no separate represented entity is named</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Section 512(n)(3) of the Federal Food, Drug, and Cosmetic Act</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>FDA’s current approval of Nexgard® (afoxolaner) Chewables as the reference listed new animal drug</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Request permission to submit an abbreviated new animal drug application (ANADA) for Afoxolaner Oral Solution 1.84% w/v, differing in dosage form from the reference listed drug</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>The proposed generic differs only in dosage form from Nexgard® chewables; Aurora seeks approval to proceed with an ANADA for afoxolaner in oral solution form under the suitability provisions of the FD&amp;C Act</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3822-0001_Citizen_Petition_from_University_of_Illinois__Coll.pdf</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>August 10, 2024</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>University of Illinois, College of Pharmacy</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Submitted by Sarfaraz K. Niazi, Ph.D., on behalf of the University of Illinois, College of Pharmacy</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>The Biologics Price Competition and Innovation Act (BPCIA); 42 USC 262(k); 21 C.F.R. § 10.30</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>FDA's prohibition against the U.S. Pharmacopeia (USP) creating monographs for biological drugs, specifically banning side-by-side analytical testing of biosimilars</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Rescind FDA’s directive to the USP prohibiting the development of monographs for biological drugs, and allow USP to create Biological Product Specifications (BPS) that define release specifications for biosimilars</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>Creating BPS would eliminate the need for costly side-by-side analytical testing with the reference product, reduce development costs, facilitate broader biosimilar access, promote harmonization, and enhance global regulatory acceptance while maintaining safety and efficacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3881-0001_Suitability_Petition_from_Zydus_Pharmaceuticals__U.pdf</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>August 13, 2024</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Zydus Pharmaceuticals (USA) Inc.</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Zydus Pharmaceuticals (USA) Inc. is submitting on its own behalf; no separate represented entity is named</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) of the FD&amp;C Act; 21 C.F.R. § 314.93; 21 C.F.R. §§ 10.20 and 10.30</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>FDA’s current limitation of the approved strengths of NUPLAZID (pimavanserin) Tablets to 10 mg and 17 mg</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Determine that Pimavanserin Tablets, 34 mg, is suitable for submission in an Abbreviated New Drug Application (ANDA)</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>The 34 mg strength matches the recommended daily dose stated in the RLD prescribing information; offering this strength in tablet form will enhance prescribing flexibility without changing dosage form or regimen, and does not raise new safety or efficacy concerns</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3905-0001_Suitability_Petition_from_Lachman_Consulting_Servi.pdf</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>August 15, 2024</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Lachman Consulting Services, Inc.</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Lachman Consulting Services, Inc. submitted the petition on behalf of an undisclosed client</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) of the FD&amp;C Act; 21 C.F.R. § 10.20; 21 C.F.R. § 10.30</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>FDA’s existing approval of Estrace® Vaginal Cream, 0.01%, as the reference listed drug, and the dosage form limitation to cream</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Determine that Estradiol Vaginal Inserts, 1 g and 2 g, are suitable for submission in an Abbreviated New Drug Application (ANDA)</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>The proposed vaginal inserts match the active ingredient and strength of the RLD cream but offer a pre-measured, easier-to-administer alternative that avoids waste and variability due to patient handling; this dosage form benefits patients with limited dexterity or vision and aligns with current dosing recommendations</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-3997-0001_Citizen_Petition_from_Aylstock__Witkin__Kreis___Ov.pdf</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>August 20, 2024</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Aylstock, Witkin, Kreis &amp; Overholtz, PLLC</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>The firm submitted the petition on its own behalf but discloses representation of consumers who purchased BPO products contaminated with benzene</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>21 C.F.R. § 10.30; 21 C.F.R. § 330.10(a)(12); 21 C.F.R. § 330.10(b); Section 501(a)(2)(B) of the FD&amp;C Act</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>FDA’s continued allowance of benzoyl peroxide (BPO) drug products on the market despite benzene contamination</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Recall and suspend sales of all benzoyl peroxide (BPO) products from the U.S. market due to the presence of benzene at levels deemed unsafe by FDA standards</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Independent lab testing showed widespread and significantly high levels of benzene in various BPO products; benzene is a Class 1 carcinogen, and its presence at levels exceeding 2 ppm violates FDA and international safety limits; the FDA has previously determined such levels to pose life-threatening risks and warrant recalls</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-4015-0001_Citizen_Petition_from_Kohl_Harrington_Redacted.pdf</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>August 22, 2024</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Kohl Harrington</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Kohl Harrington is submitting on his own behalf; no separate represented entity is named</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>5 U.S.C. § 552 (Freedom of Information Act); 21 C.F.R. § 10.30(b); 21 C.F.R. §§ 25.30 and 25.34</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>FDA-CVM’s failure to publicly post calendar records of employee Charlotte Conway despite likely being subject to multiple FOIA requests</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Comply with FOIA by posting calendar records for FDA-CVM employee Charlotte Conway (covering July 1–31, 2024) on the FDA FOIA Reading Room website</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>The FOIA requires agencies to publicly post records requested three or more times or likely to be requested again; failure to do so violates statutory obligations and undermines transparency</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-4126-0001_Suitability_Petition_from_Aurora_Pharmaceutical__I.pdf</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>August 28, 2024</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Aurora Pharmaceutical, Inc.</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Aurora Pharmaceutical, Inc. is submitting on its own behalf; no separate represented entity is named</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Section 512(n)(3) of the Federal Food, Drug, and Cosmetic Act; 21 C.F.R. § 25.30(h); 21 C.F.R. § 25.15</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>FDA’s current approval of Metacam® (meloxicam) Oral Suspension in 0.5 mg/mL and 1.5 mg/mL strengths as the reference listed new animal drug (RLNAD)</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Allow submission of an ANADA for Meloxicam Oral Solution 3 mg/mL, a higher strength and different dosage form intended for dogs over 10 lbs.</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>The proposed solution offers improved dosing accuracy and ease of administration for large dogs compared to the current suspension that requires shaking; the higher concentration reduces dosing volume, enhancing compliance without compromising safety based on prior toxicology data</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-4134-0001_Suitability_Petition_from_Pharmobedient_Consulting.pdf</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>August 24, 2024</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Pharmobedient Consulting, LLC</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Pharmobedient Consulting, LLC is submitting on its own behalf; no separate represented entity is named</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) of the FD&amp;C Act; 21 C.F.R. §§ 10.20, 10.30, 314.93; 21 C.F.R. § 25.31</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>FDA’s current limitation of approved Diclofenac Potassium tablet strengths to 25 mg and 50 mg</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Determine that Diclofenac Potassium Tablets, 37.5 mg, is suitable for submission in an Abbreviated New Drug Application (ANDA)</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>The 37.5 mg strength offers physicians greater dosing flexibility, enabling individualized treatment plans and lower effective dosing options; it remains bioequivalent to existing strengths and introduces no new concerns of safety or efficacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>FDA-2024-P-4135-0001_Suitability_Petition_from_Fresenius_Kabi_USA__LLC.pdf</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>August 27, 2024</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Fresenius Kabi USA, LLC</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Fresenius Kabi USA, LLC is submitting on its own behalf; no separate represented entity is named</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Section 505(j)(2)(C) of the FD&amp;C Act; 21 C.F.R. § 314.93; 21 C.F.R. §§ 10.20 and 10.30</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>FDA’s current approval of Vasopressin in 0.9% Sodium Chloride Injection only in 20 units/100 mL and 40 units/100 mL strengths</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Determine that Vasopressin in 0.9% Sodium Chloride Injection, 50 units/50 mL (1 unit/mL) in a single-dose ready-to-use container is suitable for submission in an Abbreviated New Drug Application (ANDA)</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>The proposed 1 unit/mL strength aligns with dosing in the approved labeling, reduces the number of IV bags needed for high-dose administrations, supports fluid-restricted patients, and complies with ASHP standards for standardized concentrations; it introduces no new safety or efficacy concerns and matches therapeutic expectations of the reference listed drug</t>
         </is>
       </c>
     </row>

</xml_diff>